<commit_message>
Petite correction du .sql et mise en forme des cellules vides du table
</commit_message>
<xml_diff>
--- a/data/Fichier Excel pour création de table-objets automatisée.xlsx
+++ b/data/Fichier Excel pour création de table-objets automatisée.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Perso\Mon-jeu-d-echec\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74016AA-727A-4C0D-A32B-44EC5E794A35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8092D3CB-BF61-472E-9AF1-9A54B8873F79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{327AC92E-88DE-44A6-9050-C07D3B569ACD}"/>
   </bookViews>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB1C851-1DE0-4AAB-89D6-C92823A5FEF3}">
   <dimension ref="A1:T834"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T65" sqref="T2:T65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -992,8 +992,8 @@
       </c>
       <c r="Q2" s="7"/>
       <c r="T2" s="8" t="str">
-        <f>"("&amp;B2&amp;", "&amp;C2&amp;", '"&amp;D2&amp;"', "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;", '"&amp;H2&amp;"', '"&amp;I2&amp;"', '"&amp;J2&amp;"', "&amp;K2&amp;", "&amp;L2&amp;"),"</f>
-        <v>(1, 8, 'white', true, false, false, 'rook', 'r1b', 'black', null, false),</v>
+        <f>"("&amp;B2&amp;", "&amp;C2&amp;", '"&amp;D2&amp;"', "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;", "&amp;IF(H2="null"," "&amp;H2&amp;","," '"&amp;H2&amp;"',")&amp;" "&amp;IF(I2="null"," "&amp;I2&amp;","," '"&amp;I2&amp;"',")&amp;" "&amp;IF(J2="null"," "&amp;J2&amp;","," '"&amp;J2&amp;"',")&amp;" "&amp;K2&amp;", "&amp;L2&amp;"),"</f>
+        <v>(1, 8, 'white', true, false, false,  'rook',  'r1b',  'black', null, false),</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1045,8 +1045,8 @@
         <v>1</v>
       </c>
       <c r="T3" s="8" t="str">
-        <f t="shared" ref="T3:T65" si="0">"("&amp;B3&amp;", "&amp;C3&amp;", '"&amp;D3&amp;"', "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", '"&amp;H3&amp;"', '"&amp;I3&amp;"', '"&amp;J3&amp;"', "&amp;K3&amp;", "&amp;L3&amp;"),"</f>
-        <v>(2, 8, 'black', true, false, false, 'knight', 'c1b', 'black', null, null),</v>
+        <f t="shared" ref="T3:T65" si="0">"("&amp;B3&amp;", "&amp;C3&amp;", '"&amp;D3&amp;"', "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;IF(H3="null"," "&amp;H3&amp;","," '"&amp;H3&amp;"',")&amp;" "&amp;IF(I3="null"," "&amp;I3&amp;","," '"&amp;I3&amp;"',")&amp;" "&amp;IF(J3="null"," "&amp;J3&amp;","," '"&amp;J3&amp;"',")&amp;" "&amp;K3&amp;", "&amp;L3&amp;"),"</f>
+        <v>(2, 8, 'black', true, false, false,  'knight',  'c1b',  'black', null, null),</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="T4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 8, 'white', true, false, false, 'bishop', 'b1b', 'black', null, null),</v>
+        <v>(3, 8, 'white', true, false, false,  'bishop',  'b1b',  'black', null, null),</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="T5" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 8, 'black', true, false, false, 'queen', 'q1b', 'black', null, null),</v>
+        <v>(4, 8, 'black', true, false, false,  'queen',  'q1b',  'black', null, null),</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="T6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 8, 'white', true, false, false, 'king', 'k1b', 'black', null, false),</v>
+        <v>(5, 8, 'white', true, false, false,  'king',  'k1b',  'black', null, false),</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="T7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 8, 'black', true, false, false, 'bishop', 'b2b', 'black', null, null),</v>
+        <v>(6, 8, 'black', true, false, false,  'bishop',  'b2b',  'black', null, null),</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="T8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 8, 'white', true, false, false, 'knight', 'c2b', 'black', null, null),</v>
+        <v>(7, 8, 'white', true, false, false,  'knight',  'c2b',  'black', null, null),</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="T9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(8, 8, 'black', true, false, false, 'rook', 'r2b', 'black', null, false),</v>
+        <v>(8, 8, 'black', true, false, false,  'rook',  'r2b',  'black', null, false),</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="T10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(1, 7, 'black', true, false, false, 'pawn', 'p1b', 'black', false, null),</v>
+        <v>(1, 7, 'black', true, false, false,  'pawn',  'p1b',  'black', false, null),</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="T11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(2, 7, 'white', true, false, false, 'pawn', 'p2b', 'black', false, null),</v>
+        <v>(2, 7, 'white', true, false, false,  'pawn',  'p2b',  'black', false, null),</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="T12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 7, 'black', true, false, false, 'pawn', 'p3b', 'black', false, null),</v>
+        <v>(3, 7, 'black', true, false, false,  'pawn',  'p3b',  'black', false, null),</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="T13" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 7, 'white', true, false, false, 'pawn', 'p4b', 'black', false, null),</v>
+        <v>(4, 7, 'white', true, false, false,  'pawn',  'p4b',  'black', false, null),</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="T14" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 7, 'black', true, false, false, 'pawn', 'p5b', 'black', false, null),</v>
+        <v>(5, 7, 'black', true, false, false,  'pawn',  'p5b',  'black', false, null),</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="T15" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 7, 'white', true, false, false, 'pawn', 'p6b', 'black', false, null),</v>
+        <v>(6, 7, 'white', true, false, false,  'pawn',  'p6b',  'black', false, null),</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="T16" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 7, 'black', true, false, false, 'pawn', 'p7b', 'black', false, null),</v>
+        <v>(7, 7, 'black', true, false, false,  'pawn',  'p7b',  'black', false, null),</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="T17" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(8, 7, 'white', true, false, false, 'pawn', 'p8b', 'black', false, null),</v>
+        <v>(8, 7, 'white', true, false, false,  'pawn',  'p8b',  'black', false, null),</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="T18" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(1, 6, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(1, 6, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="T19" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(2, 6, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(2, 6, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="T20" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 6, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(3, 6, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="T21" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 6, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(4, 6, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
       </c>
       <c r="T22" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 6, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(5, 6, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="T23" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 6, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(6, 6, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="T24" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 6, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(7, 6, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="T25" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(8, 6, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(8, 6, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2402,7 +2402,7 @@
       </c>
       <c r="T26" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(1, 5, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(1, 5, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="T27" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(2, 5, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(2, 5, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="T28" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 5, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(3, 5, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="T29" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 5, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(4, 5, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="T30" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 5, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(5, 5, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="T31" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 5, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(6, 5, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="T32" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 5, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(7, 5, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
       </c>
       <c r="T33" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(8, 5, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(8, 5, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,7 +2874,7 @@
       </c>
       <c r="T34" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(1, 4, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(1, 4, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="T35" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(2, 4, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(2, 4, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="T36" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 4, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(3, 4, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="T37" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 4, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(4, 4, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="T38" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 4, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(5, 4, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3169,7 +3169,7 @@
       </c>
       <c r="T39" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 4, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(6, 4, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="T40" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 4, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(7, 4, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
       </c>
       <c r="T41" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(8, 4, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(8, 4, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="T42" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(1, 3, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(1, 3, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="T43" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(2, 3, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(2, 3, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3464,7 +3464,7 @@
       </c>
       <c r="T44" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 3, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(3, 3, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="T45" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 3, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(4, 3, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3582,7 +3582,7 @@
       </c>
       <c r="T46" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 3, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(5, 3, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="T47" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 3, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(6, 3, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3700,7 +3700,7 @@
       </c>
       <c r="T48" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 3, 'black', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(7, 3, 'black', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="T49" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(8, 3, 'white', false, false, false, 'null', 'null', 'null', null, null),</v>
+        <v>(8, 3, 'white', false, false, false,  null,  null,  null, null, null),</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="T50" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(1, 2, 'white', true, false, false, 'pawn', 'p1w', 'white', false, null),</v>
+        <v>(1, 2, 'white', true, false, false,  'pawn',  'p1w',  'white', false, null),</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3877,7 +3877,7 @@
       </c>
       <c r="T51" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(2, 2, 'black', true, false, false, 'pawn', 'p2w', 'white', false, null),</v>
+        <v>(2, 2, 'black', true, false, false,  'pawn',  'p2w',  'white', false, null),</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="T52" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 2, 'white', true, false, false, 'pawn', 'p3w', 'white', false, null),</v>
+        <v>(3, 2, 'white', true, false, false,  'pawn',  'p3w',  'white', false, null),</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="T53" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 2, 'black', true, false, false, 'pawn', 'p4w', 'white', false, null),</v>
+        <v>(4, 2, 'black', true, false, false,  'pawn',  'p4w',  'white', false, null),</v>
       </c>
     </row>
     <row r="54" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="T54" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 2, 'white', true, false, false, 'pawn', 'p5w', 'white', false, null),</v>
+        <v>(5, 2, 'white', true, false, false,  'pawn',  'p5w',  'white', false, null),</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4112,7 +4112,7 @@
       </c>
       <c r="T55" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 2, 'black', true, false, false, 'pawn', 'p6w', 'white', false, null),</v>
+        <v>(6, 2, 'black', true, false, false,  'pawn',  'p6w',  'white', false, null),</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="T56" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 2, 'white', true, false, false, 'pawn', 'p7w', 'white', false, null),</v>
+        <v>(7, 2, 'white', true, false, false,  'pawn',  'p7w',  'white', false, null),</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="T57" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(8, 2, 'black', true, false, false, 'pawn', 'p8w', 'white', false, null),</v>
+        <v>(8, 2, 'black', true, false, false,  'pawn',  'p8w',  'white', false, null),</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="T58" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(1, 1, 'black', true, false, false, 'rook', 'r1w', 'white', null, false),</v>
+        <v>(1, 1, 'black', true, false, false,  'rook',  'r1w',  'white', null, false),</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4344,7 +4344,7 @@
       </c>
       <c r="T59" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(2, 1, 'white', true, false, false, 'knight', 'c1w', 'white', null, null),</v>
+        <v>(2, 1, 'white', true, false, false,  'knight',  'c1w',  'white', null, null),</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4402,7 +4402,7 @@
       </c>
       <c r="T60" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(3, 1, 'black', true, false, false, 'bishop', 'b1w', 'white', null, null),</v>
+        <v>(3, 1, 'black', true, false, false,  'bishop',  'b1w',  'white', null, null),</v>
       </c>
     </row>
     <row r="61" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4460,7 +4460,7 @@
       </c>
       <c r="T61" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(4, 1, 'white', true, false, false, 'queen', 'q1w', 'white', null, null),</v>
+        <v>(4, 1, 'white', true, false, false,  'queen',  'q1w',  'white', null, null),</v>
       </c>
     </row>
     <row r="62" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4518,7 +4518,7 @@
       </c>
       <c r="T62" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(5, 1, 'black', true, false, false, 'king', 'k1w', 'white', null, false),</v>
+        <v>(5, 1, 'black', true, false, false,  'king',  'k1w',  'white', null, false),</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4576,7 +4576,7 @@
       </c>
       <c r="T63" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(6, 1, 'white', true, false, false, 'bishop', 'b2w', 'white', null, null),</v>
+        <v>(6, 1, 'white', true, false, false,  'bishop',  'b2w',  'white', null, null),</v>
       </c>
     </row>
     <row r="64" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
       </c>
       <c r="T64" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>(7, 1, 'black', true, false, false, 'knight', 'c2w', 'white', null, null),</v>
+        <v>(7, 1, 'black', true, false, false,  'knight',  'c2w',  'white', null, null),</v>
       </c>
     </row>
     <row r="65" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4691,8 +4691,8 @@
         <v>5</v>
       </c>
       <c r="T65" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>(8, 1, 'white', true, false, false, 'rook', 'r2w', 'white', null, false),</v>
+        <f>"("&amp;B65&amp;", "&amp;C65&amp;", '"&amp;D65&amp;"', "&amp;E65&amp;", "&amp;F65&amp;", "&amp;G65&amp;", "&amp;IF(H65="null"," "&amp;H65&amp;","," '"&amp;H65&amp;"',")&amp;" "&amp;IF(I65="null"," "&amp;I65&amp;","," '"&amp;I65&amp;"',")&amp;" "&amp;IF(J65="null"," "&amp;J65&amp;","," '"&amp;J65&amp;"',")&amp;" "&amp;K65&amp;", "&amp;L65&amp;");"</f>
+        <v>(8, 1, 'white', true, false, false,  'rook',  'r2w',  'white', null, false);</v>
       </c>
     </row>
     <row r="66" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mise en pause du SetTimeout et j'ai fait bouger les pions, un peu...
</commit_message>
<xml_diff>
--- a/data/Fichier Excel pour création de table-objets automatisée.xlsx
+++ b/data/Fichier Excel pour création de table-objets automatisée.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Perso\Mon-jeu-d-echec\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8092D3CB-BF61-472E-9AF1-9A54B8873F79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4204FA0-85A8-474D-B1B8-864C8F7BC06A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{327AC92E-88DE-44A6-9050-C07D3B569ACD}"/>
   </bookViews>
@@ -876,7 +876,7 @@
   <dimension ref="A1:T834"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T65" sqref="T2:T65"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="8" t="str">
-        <f t="shared" ref="T3:T65" si="0">"("&amp;B3&amp;", "&amp;C3&amp;", '"&amp;D3&amp;"', "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;IF(H3="null"," "&amp;H3&amp;","," '"&amp;H3&amp;"',")&amp;" "&amp;IF(I3="null"," "&amp;I3&amp;","," '"&amp;I3&amp;"',")&amp;" "&amp;IF(J3="null"," "&amp;J3&amp;","," '"&amp;J3&amp;"',")&amp;" "&amp;K3&amp;", "&amp;L3&amp;"),"</f>
+        <f t="shared" ref="T3:T64" si="0">"("&amp;B3&amp;", "&amp;C3&amp;", '"&amp;D3&amp;"', "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;IF(H3="null"," "&amp;H3&amp;","," '"&amp;H3&amp;"',")&amp;" "&amp;IF(I3="null"," "&amp;I3&amp;","," '"&amp;I3&amp;"',")&amp;" "&amp;IF(J3="null"," "&amp;J3&amp;","," '"&amp;J3&amp;"',")&amp;" "&amp;K3&amp;", "&amp;L3&amp;"),"</f>
         <v>(2, 8, 'black', true, false, false,  'knight',  'c1b',  'black', null, null),</v>
       </c>
     </row>

</xml_diff>